<commit_message>
Update notebooks which uses old scaled amplitudes
</commit_message>
<xml_diff>
--- a/Data/Ne phase shift summary, 2018-10-24.xlsx
+++ b/Data/Ne phase shift summary, 2018-10-24.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daehyun/Documents/FERMI 20144077 Ueda/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DFFF63A-3441-0246-9DB5-E4E264CCD073}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313655ED-18ED-B34E-9448-65E8BB8B214F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41540" yWindow="2380" windowWidth="27640" windowHeight="16940" activeTab="7" xr2:uid="{B4E175A0-AA5B-DD4F-ABF8-917E44E023B1}"/>
+    <workbookView xWindow="4280" yWindow="1440" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{B4E175A0-AA5B-DD4F-ABF8-917E44E023B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Exp, β1 shift (neglected p)" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="8">
   <si>
     <t>Photon (eV)</t>
   </si>
@@ -122,60 +122,9 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="25">
     <dxf>
       <numFmt numFmtId="165" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
     <dxf>
       <font>
@@ -218,16 +167,70 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="165" formatCode="0.000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -247,20 +250,20 @@
   <autoFilter ref="A1:D5" xr:uid="{6D74ACF4-E411-B345-B3D4-342AC5AB0EA9}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{BF9BA022-C877-324C-BD27-88B738C67DF6}" name="Dataset"/>
-    <tableColumn id="2" xr3:uid="{296E6397-31C6-A141-BDAB-76ECF5F2638B}" name="Photon (eV)" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{339BED27-650B-004B-B3B8-506926E9C34E}" name="Phase shift (rad)" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{8E11364B-817B-EA42-8FCB-D75C639D189A}" name="Phase shift error (rad)" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{296E6397-31C6-A141-BDAB-76ECF5F2638B}" name="Photon (eV)" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{339BED27-650B-004B-B3B8-506926E9C34E}" name="Phase shift (rad)" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{8E11364B-817B-EA42-8FCB-D75C639D189A}" name="Phase shift error (rad)" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E7628902-5ADA-8644-BE2B-9F2E566673ED}" name="Table2" displayName="Table2" ref="A1:B4" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E7628902-5ADA-8644-BE2B-9F2E566673ED}" name="Table2" displayName="Table2" ref="A1:B4" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="A1:B4" xr:uid="{BBF55799-FC57-7044-B53A-1DF242851D61}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{0D46EFD2-9E8F-774E-8631-F35367489956}" name="Photon (eV)" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{89736DC9-36C6-594F-BD15-4AB70B3B4C71}" name="Phase shift (rad)" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{0D46EFD2-9E8F-774E-8631-F35367489956}" name="Photon (eV)" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{89736DC9-36C6-594F-BD15-4AB70B3B4C71}" name="Phase shift (rad)" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -271,21 +274,22 @@
   <autoFilter ref="A1:D5" xr:uid="{577EA140-B139-C248-ABFA-09DBAB4CB3D8}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{AAD708EB-5FB4-F246-A880-25E0D63F5CDC}" name="Dataset"/>
-    <tableColumn id="2" xr3:uid="{55F5FA46-A76B-0A49-BF11-D5E7C448BDB2}" name="Photon (eV)" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{AEBAE0BA-5796-9A41-9AA9-3C910AA4818E}" name="Phase shift (rad)" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{1426D587-9A15-4B46-8C4A-70A507380800}" name="Phase shift error (rad)" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{55F5FA46-A76B-0A49-BF11-D5E7C448BDB2}" name="Photon (eV)" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{AEBAE0BA-5796-9A41-9AA9-3C910AA4818E}" name="Phase shift (rad)" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{1426D587-9A15-4B46-8C4A-70A507380800}" name="Phase shift error (rad)" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{8D256131-175E-6149-B3B1-A0D4FCFC291A}" name="Table35691011" displayName="Table35691011" ref="A1:C5" totalsRowShown="0">
-  <autoFilter ref="A1:C5" xr:uid="{73935FFF-CBB2-B141-AF39-9C2E8C3DA6A0}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{8D256131-175E-6149-B3B1-A0D4FCFC291A}" name="Table35691011" displayName="Table35691011" ref="A1:D5" totalsRowShown="0">
+  <autoFilter ref="A1:D5" xr:uid="{73935FFF-CBB2-B141-AF39-9C2E8C3DA6A0}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{BC27FC44-984A-714F-AA1D-EAD4ABF94A57}" name="Dataset"/>
-    <tableColumn id="2" xr3:uid="{AEE4EBEC-8339-AE41-9AA1-9CF878A859BC}" name="Photon (eV)" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{3E5A7168-C73A-0F41-A052-11C5E0405068}" name="Phase shift (rad)" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{AEE4EBEC-8339-AE41-9AA1-9CF878A859BC}" name="Photon (eV)" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{3E5A7168-C73A-0F41-A052-11C5E0405068}" name="Phase shift (rad)" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{791A8267-0C6A-8A4D-9A21-04047018AD57}" name="Phase shift error (rad)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -296,8 +300,8 @@
   <autoFilter ref="A1:C5" xr:uid="{C73CAA9B-6FC7-3E4A-A9B7-E67E3433ECCB}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{35B85E09-59DF-814C-AF8D-96D5533CB148}" name="Dataset"/>
-    <tableColumn id="2" xr3:uid="{0E71D4C9-E296-5541-B75F-13D702A211E7}" name="Photon (eV)" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{F232D8CA-C70C-E843-97D8-37A2BC2B683A}" name="Phase shift (rad)" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{0E71D4C9-E296-5541-B75F-13D702A211E7}" name="Photon (eV)" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{F232D8CA-C70C-E843-97D8-37A2BC2B683A}" name="Phase shift (rad)" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -308,8 +312,8 @@
   <autoFilter ref="A1:C5" xr:uid="{538281E0-3FFA-0C46-9A79-FA287D8B3F17}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E9950D06-B9BB-F94A-A58D-48DC71797192}" name="Dataset"/>
-    <tableColumn id="2" xr3:uid="{A99235E1-2CB2-0948-ACBA-772E5E386FEF}" name="Photon (eV)" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{FBE77423-96CD-A546-A133-4BC28CD071E8}" name="Phase shift (rad)" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{A99235E1-2CB2-0948-ACBA-772E5E386FEF}" name="Photon (eV)" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{FBE77423-96CD-A546-A133-4BC28CD071E8}" name="Phase shift (rad)" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -320,8 +324,8 @@
   <autoFilter ref="A1:C5" xr:uid="{DDBC1269-F993-D746-9B8E-BF297C71F660}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{4DFDF99F-A4FE-8E4C-9405-C4DD10C69706}" name="Dataset"/>
-    <tableColumn id="2" xr3:uid="{87078886-BAC9-6446-BFFD-DC40F9C4F907}" name="Photon (eV)" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{A727CA21-79F4-AE4D-BD14-E5C115ED8FF1}" name="Phase shift (rad)" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{87078886-BAC9-6446-BFFD-DC40F9C4F907}" name="Photon (eV)" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{A727CA21-79F4-AE4D-BD14-E5C115ED8FF1}" name="Phase shift (rad)" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -332,8 +336,8 @@
   <autoFilter ref="A1:C5" xr:uid="{9FCDADA2-0B84-C545-AB2A-97845DAEDADF}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{B0E87C81-9DEB-C443-8FCB-6ED2DF9546AF}" name="Dataset"/>
-    <tableColumn id="2" xr3:uid="{AFC2E3D0-A2BA-D245-8B03-A4B41250A0F3}" name="Photon (eV)" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{E9221722-CEDB-7049-8A24-59C4406DE9EE}" name="Phase shift (rad)" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{AFC2E3D0-A2BA-D245-8B03-A4B41250A0F3}" name="Photon (eV)" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{E9221722-CEDB-7049-8A24-59C4406DE9EE}" name="Phase shift (rad)" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -344,8 +348,8 @@
   <autoFilter ref="A1:C5" xr:uid="{341908F9-2B9B-604A-90AD-5DD5248F9856}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{845779A6-D71D-C949-89DD-3AA8B8AC6CE1}" name="Dataset"/>
-    <tableColumn id="2" xr3:uid="{57847AA9-10E0-8540-AA0D-15FD76F567D5}" name="Photon (eV)" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{C8D03E42-77C1-3749-97A6-70E624BCBCA0}" name="Phase shift (rad)" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{57847AA9-10E0-8540-AA0D-15FD76F567D5}" name="Photon (eV)" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{C8D03E42-77C1-3749-97A6-70E624BCBCA0}" name="Phase shift (rad)" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -355,8 +359,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E289F6C4-2F08-0A4C-94A9-3CCD59E85C54}" name="Table1" displayName="Table1" ref="A1:B32" totalsRowShown="0">
   <autoFilter ref="A1:B32" xr:uid="{3843A1F0-128B-6640-BBB7-7DD5A0E5F508}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{E5ED8E81-F732-BF45-A565-DD6729D9101A}" name="Photon (eV)" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{08E89415-8A10-9C44-BE64-964FD688CFD8}" name="Phase shift (rad)" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{E5ED8E81-F732-BF45-A565-DD6729D9101A}" name="Photon (eV)" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{08E89415-8A10-9C44-BE64-964FD688CFD8}" name="Phase shift (rad)" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -809,7 +813,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="D5" sqref="D1:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -903,19 +907,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4524FEDC-1ABC-304E-BC65-F3F5933704B8}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13.1640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="17.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -925,8 +930,11 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -934,18 +942,28 @@
         <v>15.9</v>
       </c>
       <c r="C2" s="1">
-        <v>1.522</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1.52</v>
+      </c>
+      <c r="D2" s="1">
+        <f>0.042</f>
+        <v>4.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2">
         <v>14.3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C3" s="1">
+        <v>-0.26700000000000002</v>
+      </c>
+      <c r="D3" s="1">
+        <v>21077.32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -953,10 +971,13 @@
         <v>19.100000000000001</v>
       </c>
       <c r="C4" s="1">
-        <v>1.3839999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1.4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3.1E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -964,7 +985,10 @@
         <v>15.9</v>
       </c>
       <c r="C5" s="1">
-        <v>1.5189999999999999</v>
+        <v>1.5149999999999999</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4.8000000000000001E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1287,7 +1311,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13AB4DBA-E8C6-A04A-9B95-62699F0AC7D0}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update data "Ne phase shift summary, 2018-10-24.xlsx" and notebook "Compare Ne beta phase shifts (summary).ipynb"
</commit_message>
<xml_diff>
--- a/Data/Ne phase shift summary, 2018-10-24.xlsx
+++ b/Data/Ne phase shift summary, 2018-10-24.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daehyun/Documents/FERMI 20144077 Ueda/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313655ED-18ED-B34E-9448-65E8BB8B214F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8997034A-9DD2-9742-9388-2CFF1BCDAC4B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4280" yWindow="1440" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{B4E175A0-AA5B-DD4F-ABF8-917E44E023B1}"/>
   </bookViews>
@@ -910,7 +910,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -955,9 +955,6 @@
       </c>
       <c r="B3" s="2">
         <v>14.3</v>
-      </c>
-      <c r="C3" s="1">
-        <v>-0.26700000000000002</v>
       </c>
       <c r="D3" s="1">
         <v>21077.32</v>

</xml_diff>